<commit_message>
modify (admin panel): add new functionality
</commit_message>
<xml_diff>
--- a/reports/guest.xlsx
+++ b/reports/guest.xlsx
@@ -14,30 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73" count="73">
-  <x:si>
-    <x:t>id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>firstName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lastName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>phone</x:t>
-  </x:si>
-  <x:si>
-    <x:t>address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>passportDetails</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dateOfBirth</x:t>
-  </x:si>
-  <x:si>
-    <x:t>discountCode</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79" count="79">
+  <x:si>
+    <x:t>First name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Last name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phone number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Passport details</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date of Birth</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Discount code</x:t>
   </x:si>
   <x:si>
     <x:t>Остап</x:t>
@@ -55,7 +52,7 @@
     <x:t>ВН 354928</x:t>
   </x:si>
   <x:si>
-    <x:t>Thu Jan 18 1990 00:00:00 GMT+0200 (Финляндия (зима))</x:t>
+    <x:t>18 : 01 : 1990</x:t>
   </x:si>
   <x:si>
     <x:t>234285</x:t>
@@ -76,7 +73,7 @@
     <x:t>ВН 259851</x:t>
   </x:si>
   <x:si>
-    <x:t>Sun Feb 24 1980 00:00:00 GMT+0200 (Финляндия (зима))</x:t>
+    <x:t>24 : 02 : 1980</x:t>
   </x:si>
   <x:si>
     <x:t>545634</x:t>
@@ -97,7 +94,7 @@
     <x:t>ВН 105378</x:t>
   </x:si>
   <x:si>
-    <x:t>Wed Mar 20 1996 00:00:00 GMT+0200 (Финляндия (зима))</x:t>
+    <x:t>20 : 03 : 1996</x:t>
   </x:si>
   <x:si>
     <x:t>Иван</x:t>
@@ -115,7 +112,7 @@
     <x:t>ВН 966710</x:t>
   </x:si>
   <x:si>
-    <x:t>Fri May 05 1978 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>05 : 05 : 1978</x:t>
   </x:si>
   <x:si>
     <x:t>Эдуард</x:t>
@@ -133,7 +130,7 @@
     <x:t>ВН 279772</x:t>
   </x:si>
   <x:si>
-    <x:t>Fri Jun 03 1988 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>03 : 06 : 1988</x:t>
   </x:si>
   <x:si>
     <x:t>305809</x:t>
@@ -154,7 +151,7 @@
     <x:t>ВН 384258</x:t>
   </x:si>
   <x:si>
-    <x:t>Thu Jul 13 1967 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>13 : 07 : 1967</x:t>
   </x:si>
   <x:si>
     <x:t>435839</x:t>
@@ -175,7 +172,7 @@
     <x:t>ВН 369927</x:t>
   </x:si>
   <x:si>
-    <x:t>Tue Aug 04 1987 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>04 : 08 : 1987</x:t>
   </x:si>
   <x:si>
     <x:t>Денис</x:t>
@@ -193,7 +190,7 @@
     <x:t>ВН 861454</x:t>
   </x:si>
   <x:si>
-    <x:t>Tue Sep 28 1976 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>28 : 09 : 1976</x:t>
   </x:si>
   <x:si>
     <x:t>Николай</x:t>
@@ -211,7 +208,7 @@
     <x:t>ВН 976009</x:t>
   </x:si>
   <x:si>
-    <x:t>Fri Oct 01 1993 00:00:00 GMT+0300 (Финляндия (лето))</x:t>
+    <x:t>01 : 10 : 1993</x:t>
   </x:si>
   <x:si>
     <x:t>Александр</x:t>
@@ -229,10 +226,31 @@
     <x:t>ВН 689592</x:t>
   </x:si>
   <x:si>
-    <x:t>Wed Nov 15 1995 00:00:00 GMT+0200 (Финляндия (зима))</x:t>
+    <x:t>15 : 11 : 1995</x:t>
   </x:si>
   <x:si>
     <x:t>095424</x:t>
+  </x:si>
+  <x:si>
+    <x:t>цу</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ук</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ку</x:t>
+  </x:si>
+  <x:si>
+    <x:t>цуацуацуацауцацуацуа цуацкккккуацуауууууууу</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23вуца</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 : 06 : 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21квцу</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -595,7 +613,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
+    <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -617,13 +635,10 @@
       <x:c r="G1" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" s="0" t="n">
-        <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>8</x:v>
@@ -643,13 +658,10 @@
       <x:c r="G2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="0" t="s">
         <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="n">
-        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>15</x:v>
@@ -669,13 +681,10 @@
       <x:c r="G3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="0" t="s">
         <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="n">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>22</x:v>
@@ -692,13 +701,10 @@
       <x:c r="F4" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="A5" s="0" t="s">
         <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" s="0" t="n">
-        <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>28</x:v>
@@ -715,13 +721,10 @@
       <x:c r="F5" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="s">
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="A6" s="0" t="s">
         <x:v>33</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" s="0" t="n">
-        <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>34</x:v>
@@ -741,13 +744,10 @@
       <x:c r="G6" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="H6" s="0" t="s">
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="A7" s="0" t="s">
         <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:8">
-      <x:c r="A7" s="0" t="n">
-        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>41</x:v>
@@ -767,13 +767,10 @@
       <x:c r="G7" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="H7" s="0" t="s">
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="A8" s="0" t="s">
         <x:v>47</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:8">
-      <x:c r="A8" s="0" t="n">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>48</x:v>
@@ -790,13 +787,10 @@
       <x:c r="F8" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="G8" s="0" t="s">
+    </x:row>
+    <x:row r="9" spans="1:7">
+      <x:c r="A9" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:8">
-      <x:c r="A9" s="0" t="n">
-        <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>54</x:v>
@@ -813,13 +807,10 @@
       <x:c r="F9" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="G9" s="0" t="s">
+    </x:row>
+    <x:row r="10" spans="1:7">
+      <x:c r="A10" s="0" t="s">
         <x:v>59</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:8">
-      <x:c r="A10" s="0" t="n">
-        <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>60</x:v>
@@ -836,13 +827,10 @@
       <x:c r="F10" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="G10" s="0" t="s">
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="0" t="s">
         <x:v>65</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:8">
-      <x:c r="A11" s="0" t="n">
-        <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>66</x:v>
@@ -862,8 +850,28 @@
       <x:c r="G11" s="0" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="H11" s="0" t="s">
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="0" t="s">
         <x:v>72</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>78</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>